<commit_message>
Update effort and uploaded RASD v 0.6.1
</commit_message>
<xml_diff>
--- a/Effort/EffortGianmarcoAccordi.xlsx
+++ b/Effort/EffortGianmarcoAccordi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianmarco Accordi\Documents\Project-INGSW2\AbboAccordiBonetti\Effort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDCD182-3074-5E4A-80C1-5D7D9874893F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C85DCB5-BF9E-4574-A0BB-D4C45FB29212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,24 +430,24 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD23"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -455,15 +455,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -471,41 +471,41 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Added RASD v 0.9.3
</commit_message>
<xml_diff>
--- a/Effort/EffortGianmarcoAccordi.xlsx
+++ b/Effort/EffortGianmarcoAccordi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianmarco Accordi\Documents\Project-INGSW2\AbboAccordiBonetti\Effort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9568BFA9-388F-44E8-8A4D-5D60A76EDF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24323201-D581-4139-9CF9-45C692A08E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -460,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,6 +508,9 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update version RASD 0.9.8.4
</commit_message>
<xml_diff>
--- a/Effort/EffortGianmarcoAccordi.xlsx
+++ b/Effort/EffortGianmarcoAccordi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianmarco Accordi\Documents\Project-INGSW2\AbboAccordiBonetti\Effort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7A8412-82E9-41B7-973A-92B1B5250B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F11CBB7-7D7A-4A51-A809-2B59B1CF2FEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,7 +511,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -519,7 +519,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,7 +528,7 @@
       </c>
       <c r="B12">
         <f>SUM(B3:B10)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>